<commit_message>
feat: add download data_mahasiswa (admin)
</commit_message>
<xml_diff>
--- a/data/Data_Mahasiswa.xlsx
+++ b/data/Data_Mahasiswa.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1002"/>
+  <dimension ref="A1:J1004"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -36486,10 +36486,8 @@
       </c>
     </row>
     <row r="1002">
-      <c r="A1002" t="inlineStr">
-        <is>
-          <t>68631551</t>
-        </is>
+      <c r="A1002" t="n">
+        <v>68631551</v>
       </c>
       <c r="B1002" t="inlineStr">
         <is>
@@ -36521,6 +36519,80 @@
       </c>
       <c r="J1002" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="n">
+        <v>93338203</v>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Ezio</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>Sistem Informasi</t>
+        </is>
+      </c>
+      <c r="D1003" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E1003" t="n">
+        <v>1</v>
+      </c>
+      <c r="F1003" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G1003" t="n">
+        <v>1</v>
+      </c>
+      <c r="H1003" t="n">
+        <v>1</v>
+      </c>
+      <c r="I1003" t="n">
+        <v>1</v>
+      </c>
+      <c r="J1003" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>83779280</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Miawaug</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>Sistem Informasi</t>
+        </is>
+      </c>
+      <c r="D1004" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E1004" t="n">
+        <v>1</v>
+      </c>
+      <c r="F1004" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G1004" t="n">
+        <v>1</v>
+      </c>
+      <c r="H1004" t="n">
+        <v>1</v>
+      </c>
+      <c r="I1004" t="n">
+        <v>1</v>
+      </c>
+      <c r="J1004" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>